<commit_message>
Updated project plan document to include WBS, Gantt Chart and Activity Definition Estimation
</commit_message>
<xml_diff>
--- a/SydneyGantt.xlsx
+++ b/SydneyGantt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s5143355\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Software Tech\Assignment\2810ICT_Assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A785340B-00A1-4041-ABE9-D874D0F4A6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57FEEE6-0D22-4E85-AE46-A27F334AF001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3900" yWindow="435" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -300,10 +300,6 @@
     <t>Handover Final Software Version</t>
   </si>
   <si>
-    <t>Software Testing
-Report</t>
-  </si>
-  <si>
     <t>Sydney Airbnb Data Analysis Project</t>
   </si>
   <si>
@@ -362,6 +358,9 @@
   </si>
   <si>
     <t>Extract review price/rating</t>
+  </si>
+  <si>
+    <t>Software Testing Report</t>
   </si>
 </sst>
 </file>
@@ -877,6 +876,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -923,9 +925,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1330,18 +1329,18 @@
   </sheetPr>
   <dimension ref="A1:BO54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection sqref="A1:BD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="52.125" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="27" width="2.75" style="1"/>
     <col min="42" max="42" width="2.75" customWidth="1"/>
@@ -1350,7 +1349,7 @@
   <sheetData>
     <row r="1" spans="1:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1359,51 +1358,51 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="11">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="J2" s="12"/>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="55"/>
       <c r="P2" s="13"/>
-      <c r="Q2" s="52" t="s">
+      <c r="Q2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="54"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="55"/>
       <c r="U2" s="14"/>
-      <c r="V2" s="56" t="s">
+      <c r="V2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="59"/>
       <c r="Z2" s="15"/>
-      <c r="AA2" s="59" t="s">
+      <c r="AA2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
+      <c r="AF2" s="61"/>
+      <c r="AG2" s="62"/>
       <c r="AH2" s="16"/>
       <c r="AI2" s="18" t="s">
         <v>4</v>
@@ -1417,22 +1416,22 @@
       <c r="AP2" s="19"/>
     </row>
     <row r="3" spans="1:67" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="51" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1459,12 +1458,12 @@
       <c r="AA3" s="7"/>
     </row>
     <row r="4" spans="1:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="64"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1647,7 +1646,7 @@
       </c>
     </row>
     <row r="5" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66">
+      <c r="A5" s="50">
         <v>1</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -2072,7 +2071,7 @@
     </row>
     <row r="25" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>37</v>
@@ -2092,7 +2091,7 @@
     </row>
     <row r="26" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>38</v>
@@ -2132,7 +2131,7 @@
     </row>
     <row r="28" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>40</v>
@@ -2152,7 +2151,7 @@
     </row>
     <row r="29" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>41</v>
@@ -2192,7 +2191,7 @@
     </row>
     <row r="31" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>43</v>
@@ -2212,7 +2211,7 @@
     </row>
     <row r="32" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="25" t="s">
         <v>44</v>
@@ -2232,7 +2231,7 @@
     </row>
     <row r="33" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="25" t="s">
         <v>45</v>
@@ -2272,7 +2271,7 @@
     </row>
     <row r="35" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="25" t="s">
         <v>47</v>
@@ -2292,7 +2291,7 @@
     </row>
     <row r="36" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="25" t="s">
         <v>48</v>
@@ -2312,7 +2311,7 @@
     </row>
     <row r="37" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="25" t="s">
         <v>49</v>
@@ -2335,7 +2334,7 @@
         <v>3.7</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="33">
         <v>32</v>
@@ -2352,10 +2351,10 @@
     </row>
     <row r="39" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="37">
         <v>32</v>
@@ -2372,7 +2371,7 @@
     </row>
     <row r="40" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" s="25" t="s">
         <v>45</v>
@@ -2392,7 +2391,7 @@
     </row>
     <row r="41" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="25" t="s">
         <v>50</v>
@@ -2432,7 +2431,7 @@
     </row>
     <row r="43" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" s="25" t="s">
         <v>52</v>
@@ -2452,7 +2451,7 @@
     </row>
     <row r="44" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" s="25" t="s">
         <v>53</v>
@@ -2532,7 +2531,7 @@
     </row>
     <row r="48" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="25" t="s">
         <v>57</v>
@@ -2552,7 +2551,7 @@
     </row>
     <row r="49" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B49" s="25" t="s">
         <v>58</v>
@@ -2635,7 +2634,7 @@
         <v>5.3</v>
       </c>
       <c r="B53" s="27" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C53" s="41">
         <v>48</v>

</xml_diff>